<commit_message>
remove table location llm output
</commit_message>
<xml_diff>
--- a/files/Tester_1.xlsx
+++ b/files/Tester_1.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>table_header_descriptor</t>
+          <t>table_header_position</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -516,27 +516,27 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Swage Dia. In Mm</t>
+          <t>Swaging Dimensions Swage Dia. In Mm</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Tail Id Top Tolerance</t>
+          <t>Tail Id Top Tolerance Mm</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Tail Id Bottom Tolerance</t>
+          <t>Tail Id Bottom Tolerance Mm</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Swaged No Go</t>
+          <t>Swaged No Go Mm</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Swaged Go</t>
+          <t>Swaged Go Mm</t>
         </is>
       </c>
     </row>
@@ -732,7 +732,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>"1 Wire, 100 Metre Coils - Can be found on the middle left position of the page"</t>
+          <t>- "1 Wire, 100 Metre Coils - Can be found on the bottom left position of the page"</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -785,7 +785,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>"1 Wire, 100 Metre Coils - Can be found on the middle left position of the page"</t>
+          <t>- "1 Wire, 100 Metre Coils - Can be found on the bottom left position of the page"</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -838,7 +838,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>"1 Wire, 100 Metre Coils - Can be found on the middle left position of the page"</t>
+          <t>- "1 Wire, 100 Metre Coils - Can be found on the bottom left position of the page"</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -891,7 +891,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>"1 Wire, 100 Metre Coils - Can be found on the middle left position of the page"</t>
+          <t>- "1 Wire, 100 Metre Coils - Can be found on the bottom left position of the page"</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -944,7 +944,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>"1 Wire, 100 Metre Coils - Can be found on the middle left position of the page"</t>
+          <t>- "1 Wire, 100 Metre Coils - Can be found on the bottom left position of the page"</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>"1 Wire, 100 Metre Coils - Can be found on the middle left position of the page"</t>
+          <t>- "1 Wire, 100 Metre Coils - Can be found on the bottom left position of the page"</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>"1 Wire, 100 Metre Coils - Can be found on the middle left position of the page"</t>
+          <t>- "1 Wire, 100 Metre Coils - Can be found on the bottom left position of the page"</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>"1 Wire, 100 Metre Coils - Can be found on the middle left position of the page"</t>
+          <t>- "1 Wire, 100 Metre Coils - Can be found on the bottom left position of the page"</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1852,7 +1852,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -2030,7 +2030,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>"Hydraulic Hose, EN853, DIN20022, SAE100R1AT Technical Data - Can be found at the bottom of the page"</t>
+          <t>- "Technical Data - Can be found on the very bottom position of the page"</t>
         </is>
       </c>
       <c r="H23" t="n">

</xml_diff>